<commit_message>
"Added a JS file with the array w/ questions"
</commit_message>
<xml_diff>
--- a/Content.xlsx
+++ b/Content.xlsx
@@ -77,9 +77,6 @@
     <t>Karim Benzema</t>
   </si>
   <si>
-    <t>Name the player that currently play with the team and is among the top 5 goal scorer of all time?</t>
-  </si>
-  <si>
     <t>How many Uefa Champions league titles does the madrid owns?</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>&lt;a href="https://www.freeiconspng.com/img/24651" title="Image from freeiconspng.com"&gt;&lt;img src="https://www.freeiconspng.com/uploads/real-madrid-logo-png-15.png" width="350" alt="PNG Transparent Image Real Madrid Logo" /&gt;&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Name a current player of the team that is ranked among the Top 5 striker of all time?</t>
   </si>
 </sst>
 </file>
@@ -122,12 +122,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,9 +149,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,84 +469,84 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>1956</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>33</v>
@@ -547,12 +554,12 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>